<commit_message>
Remove some string getter from enum + Master excel now uses id as key value + Change script to use id
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterAchievement.xlsx
+++ b/Assets/Data/Excel/MasterAchievement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7C5326-062A-4074-8014-B36A951C21F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247EC1E8-FAD4-4079-8BEE-4024BBF3A385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>achievementType</t>
-  </si>
-  <si>
     <t>ps4ID</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>isHidden</t>
-  </si>
-  <si>
-    <t>Clear_Game_Once</t>
   </si>
   <si>
     <t>achievement_100</t>
@@ -418,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
@@ -436,12 +430,12 @@
     <col min="8" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -458,33 +452,27 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>90000</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
       </c>
       <c r="D2">
         <v>-1</v>
       </c>
-      <c r="E2">
-        <v>-1</v>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="b">
+        <v>6</v>
+      </c>
+      <c r="G2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Achievement update (still need to test locally/Steam) + main scenes are automatically added when in correct folder
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterAchievement.xlsx
+++ b/Assets/Data/Excel/MasterAchievement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247EC1E8-FAD4-4079-8BEE-4024BBF3A385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3D400-FB2B-45E8-A8CD-0B0707B4D568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -48,9 +48,6 @@
     <t>steamID</t>
   </si>
   <si>
-    <t>nameLocalizationKey</t>
-  </si>
-  <si>
     <t>isHidden</t>
   </si>
   <si>
@@ -60,14 +57,36 @@
     <t>achievementName</t>
   </si>
   <si>
-    <t>ClearGameOnce</t>
+    <t>targetKey</t>
+  </si>
+  <si>
+    <t>targetRequiredAmount</t>
+  </si>
+  <si>
+    <t>GoodEnding</t>
+  </si>
+  <si>
+    <t>BadEnding</t>
+  </si>
+  <si>
+    <t>targetKey with value -1 will be completed when called.</t>
+  </si>
+  <si>
+    <t>This is normally for achievement which does not need to be compared with required amount.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,15 +95,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,15 +116,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,15 +469,16 @@
     <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -450,15 +493,29 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>90000</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -467,12 +524,52 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="b">
+        <v>5</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>90001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make sure all statebase checks for Pause state machine OnEnter and OnExit + glossary now updates by event for inventory(supposedly achievement too which is not done) + able to save/load inventory(need more testing) + steamworks for avatar + animator state + extentions
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterAchievement.xlsx
+++ b/Assets/Data/Excel/MasterAchievement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3D400-FB2B-45E8-A8CD-0B0707B4D568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0758505-E112-4475-B8FB-4A3915E8890F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -51,9 +51,6 @@
     <t>isHidden</t>
   </si>
   <si>
-    <t>achievement_100</t>
-  </si>
-  <si>
     <t>achievementName</t>
   </si>
   <si>
@@ -73,13 +70,25 @@
   </si>
   <si>
     <t>This is normally for achievement which does not need to be compared with required amount.</t>
+  </si>
+  <si>
+    <t>ClearGameOnce</t>
+  </si>
+  <si>
+    <t>goodEnding_90000</t>
+  </si>
+  <si>
+    <t>badEnding_90001</t>
+  </si>
+  <si>
+    <t>clearGame_99000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,8 +103,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +121,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -132,15 +153,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -454,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,7 +490,7 @@
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.88671875" customWidth="1"/>
@@ -478,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -493,13 +517,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -515,7 +539,7 @@
         <v>90000</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -524,7 +548,7 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -536,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -552,7 +576,7 @@
         <v>90001</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -561,7 +585,7 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -570,6 +594,32 @@
         <v>-1</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>99000</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
It should now fixed the strafing slowdown. It will only slowdown if you pressed the back button or any button with combination with back button.
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterAchievement.xlsx
+++ b/Assets/Data/Excel/MasterAchievement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0758505-E112-4475-B8FB-4A3915E8890F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D32EB3-40E6-4CA8-A0C2-87807E386D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>isHidden</t>
   </si>
   <si>
-    <t>achievementName</t>
-  </si>
-  <si>
     <t>targetKey</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>clearGame_99000</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -517,13 +517,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -539,7 +539,7 @@
         <v>90000</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -548,7 +548,7 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -576,7 +576,7 @@
         <v>90001</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -585,7 +585,7 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -602,7 +602,7 @@
         <v>99000</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>-1</v>
@@ -611,7 +611,7 @@
         <v>-1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Ongoing definiton to enumType
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterAchievement.xlsx
+++ b/Assets/Data/Excel/MasterAchievement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D32EB3-40E6-4CA8-A0C2-87807E386D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50EBD75-FDBC-4AB4-B59B-0E83645018B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -57,21 +57,12 @@
     <t>targetRequiredAmount</t>
   </si>
   <si>
-    <t>GoodEnding</t>
-  </si>
-  <si>
-    <t>BadEnding</t>
-  </si>
-  <si>
     <t>targetKey with value -1 will be completed when called.</t>
   </si>
   <si>
     <t>This is normally for achievement which does not need to be compared with required amount.</t>
   </si>
   <si>
-    <t>ClearGameOnce</t>
-  </si>
-  <si>
     <t>goodEnding_90000</t>
   </si>
   <si>
@@ -82,6 +73,21 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Good_Ending</t>
+  </si>
+  <si>
+    <t>Bad_Ending</t>
+  </si>
+  <si>
+    <t>Clear_Game_Once</t>
+  </si>
+  <si>
+    <t>All_Achievements</t>
+  </si>
+  <si>
+    <t>allAchievement_99999</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -523,7 +529,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -539,7 +545,7 @@
         <v>90000</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -548,7 +554,7 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -560,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -576,7 +582,7 @@
         <v>90001</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -585,7 +591,7 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -602,17 +608,17 @@
         <v>99000</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="2" t="b">
         <v>0</v>
       </c>
@@ -620,6 +626,32 @@
         <v>-1</v>
       </c>
       <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>99999</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create a definition for converting excel to enum(removed the editor script)
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterAchievement.xlsx
+++ b/Assets/Data/Excel/MasterAchievement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D68A41-B6C2-40B4-8D69-357531C59848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6C5E80-CE2E-4A56-BEB1-5281A68E61D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>lockMaster_91000</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,16 +554,13 @@
         <v>90000</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>-1</v>
       </c>
       <c r="D2">
         <v>-1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -588,7 +588,7 @@
         <v>90001</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -597,7 +597,7 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -611,10 +611,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>91000</v>
+        <v>90002</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -623,67 +623,93 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>10201</v>
+        <v>-1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>99000</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
+      <c r="A5">
+        <v>91000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>10201</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="2">
+        <v>99000</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>99999</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
-        <v>-1</v>
-      </c>
-      <c r="D6">
-        <v>-1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>-1</v>
-      </c>
-      <c r="H6">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>

</xml_diff>